<commit_message>
Checkpoint: Reverted combined_script.py to last committed version
</commit_message>
<xml_diff>
--- a/web_app/uploads/Lakshmi_Narasimhan_20250501_120130.xlsx
+++ b/web_app/uploads/Lakshmi_Narasimhan_20250501_120130.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narasimhan/workarea/betterhome/web_app/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6E79B0-A186-CF4C-AC91-70812AF33C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D53A0E-07A4-B64B-8E7E-2C6361EF0ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>Hob (built-in) - placed inside</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>100</t>
@@ -598,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -799,56 +796,56 @@
       <c r="Q2" t="s">
         <v>60</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
         <v>61</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" t="s">
         <v>62</v>
       </c>
-      <c r="T2" t="s">
-        <v>56</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>63</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>64</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" t="s">
         <v>65</v>
       </c>
-      <c r="Y2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL2" t="s">
         <v>68</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>69</v>
       </c>
       <c r="AM2" t="s">
         <v>58</v>
@@ -860,13 +857,13 @@
         <v>56</v>
       </c>
       <c r="AP2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AQ2" t="s">
         <v>56</v>
       </c>
       <c r="AS2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AT2" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
fix duplicates and better features
</commit_message>
<xml_diff>
--- a/web_app/uploads/Lakshmi_Narasimhan_20250501_120130.xlsx
+++ b/web_app/uploads/Lakshmi_Narasimhan_20250501_120130.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narasimhan/workarea/betterhome/web_app/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D53A0E-07A4-B64B-8E7E-2C6361EF0ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A65521C-1C12-B048-BE14-433E5D260BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -797,7 +797,7 @@
         <v>60</v>
       </c>
       <c r="R2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S2" t="s">
         <v>61</v>

</xml_diff>